<commit_message>
read to product list wf ,produc stock wf and kill process workflows added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -162,15 +162,9 @@
     <t>ProductListExcelPath</t>
   </si>
   <si>
-    <t>C:\Users\GAMZE\Desktop\Ürün Stok Projesi\Ürün Listesi.xlsx</t>
-  </si>
-  <si>
     <t>StockExcelPath</t>
   </si>
   <si>
-    <t>C:\Users\GAMZE\Desktop\Ürün Stok Projesi\Stok Excel.xlsx</t>
-  </si>
-  <si>
     <t>EmailTo</t>
   </si>
   <si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>excel</t>
+  </si>
+  <si>
+    <t>C:\Users\GAMZE\Desktop\Ürün Stok Projesi\ProductList.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\GAMZE\Desktop\Ürün Stok Projesi\ProductStock.xlsx</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -643,32 +643,32 @@
       <c r="A5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
-        <v>47</v>
+      <c r="B5" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
ıtems added with add queue item
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -92,95 +92,91 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>ProductStockStatus</t>
+  </si>
+  <si>
+    <t>ProductListExcelPath</t>
+  </si>
+  <si>
+    <t>StockExcelPath</t>
+  </si>
+  <si>
+    <t>EmailTo</t>
+  </si>
+  <si>
+    <t>esra.arnus@gmail.com</t>
+  </si>
+  <si>
+    <t>KillProcess</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>C:\Users\GAMZE\Desktop\Ürün Stok Projesi\ProductList.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\GAMZE\Desktop\Ürün Stok Projesi\ProductStock.xlsx</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProductStockStatus</t>
-  </si>
-  <si>
-    <t>My Workspace</t>
-  </si>
-  <si>
-    <t>ProductListExcelPath</t>
-  </si>
-  <si>
-    <t>StockExcelPath</t>
-  </si>
-  <si>
-    <t>EmailTo</t>
-  </si>
-  <si>
-    <t>esra.arnus@gmail.com</t>
-  </si>
-  <si>
-    <t>KillProcess</t>
-  </si>
-  <si>
-    <t>excel</t>
-  </si>
-  <si>
-    <t>C:\Users\GAMZE\Desktop\Ürün Stok Projesi\ProductList.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\GAMZE\Desktop\Ürün Stok Projesi\ProductStock.xlsx</t>
   </si>
 </sst>
 </file>
@@ -550,7 +546,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,7 +557,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -608,10 +604,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -619,13 +615,11 @@
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="28.8">
@@ -641,34 +635,34 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1724,18 +1718,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1759,7 +1753,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1781,7 +1775,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1792,7 +1786,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1803,53 +1797,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2851,7 +2845,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
process end process edited
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -173,16 +173,16 @@
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>ReportExcelPath</t>
-  </si>
-  <si>
-    <t>C:\Users\GAMZE\Documents\UiPath\ProductStockStatus\Data\Output\Report.xlsx</t>
-  </si>
-  <si>
     <t>C:\Users\GAMZE\Documents\UiPath\ProductStockStatus\Data\Input\ProductList.xlsx</t>
   </si>
   <si>
     <t>C:\Users\GAMZE\Documents\UiPath\ProductStockStatus\Data\Input\ProductStock.xlsx</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>REF Ödev</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -644,7 +644,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -652,7 +652,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -665,18 +665,18 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>